<commit_message>
Fixed all - column names problems and desafio1.json problems
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -146,9 +146,6 @@
     <t xml:space="preserve">plano_id</t>
   </si>
   <si>
-    <t xml:space="preserve">nome</t>
-  </si>
-  <si>
     <t xml:space="preserve">cancao_id</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t xml:space="preserve">seguindo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">álbum</t>
   </si>
   <si>
     <t xml:space="preserve">cancoes_id</t>
@@ -238,7 +238,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -266,11 +266,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -356,7 +351,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,7 +440,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,24 +512,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -852,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -862,7 +841,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="25.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="11.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="10.38"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="20" width="9.14"/>
@@ -888,7 +867,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>4</v>
@@ -899,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="24"/>
       <c r="AMJ2" s="24"/>
@@ -917,7 +896,7 @@
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="31" t="n">
         <v>1</v>
@@ -973,7 +952,7 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
       <c r="F7" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="31" t="n">
         <v>13</v>
@@ -984,10 +963,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C8" s="31"/>
       <c r="F8" s="30"/>
@@ -1033,7 +1012,7 @@
       </c>
       <c r="C11" s="31"/>
       <c r="F11" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="31" t="n">
         <v>4</v>
@@ -1070,7 +1049,7 @@
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="F14" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="31" t="n">
         <v>3</v>
@@ -1081,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>2</v>
@@ -1109,7 +1088,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="29"/>
@@ -1131,7 +1110,7 @@
         <v>35</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="34"/>
       <c r="F17" s="33"/>
@@ -1149,11 +1128,11 @@
         <v>20</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="34"/>
       <c r="F18" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="33"/>
@@ -1170,14 +1149,14 @@
         <v>45</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="34"/>
       <c r="F19" s="28" t="s">
         <v>0</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="33"/>
       <c r="AMJ19" s="24"/>
@@ -1192,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20" s="33"/>
       <c r="AMJ20" s="24"/>
@@ -1204,7 +1183,7 @@
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="F21" s="38"/>
-      <c r="G21" s="40" t="n">
+      <c r="G21" s="31" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1213,15 +1192,15 @@
         <v>22</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+        <v>44</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="38"/>
-      <c r="G22" s="40" t="n">
+      <c r="G22" s="31" t="n">
         <v>3</v>
       </c>
       <c r="H22" s="24"/>
@@ -1235,7 +1214,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
@@ -1243,7 +1222,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H23" s="24"/>
       <c r="AMJ23" s="24"/>
@@ -1256,12 +1235,12 @@
         <v>29</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="38"/>
-      <c r="G24" s="40" t="n">
+      <c r="G24" s="31" t="n">
         <v>3</v>
       </c>
       <c r="H24" s="24"/>
@@ -1275,7 +1254,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -1283,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H25" s="24"/>
       <c r="AMJ25" s="24"/>
@@ -1296,12 +1275,12 @@
         <v>34</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="38"/>
-      <c r="G26" s="40" t="n">
+      <c r="G26" s="31" t="n">
         <v>1</v>
       </c>
       <c r="H26" s="24"/>
@@ -1315,15 +1294,15 @@
         <v>37</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+        <v>46</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="38" t="n">
         <v>4</v>
       </c>
       <c r="G27" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H27" s="24"/>
       <c r="AMJ27" s="24"/>
@@ -1332,9 +1311,9 @@
       <c r="A28" s="35"/>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="42"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="33"/>
       <c r="H28" s="24"/>
       <c r="AMJ28" s="24"/>
@@ -1354,7 +1333,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>22</v>
@@ -1371,9 +1350,9 @@
         <v>50</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="42"/>
+        <v>42</v>
+      </c>
+      <c r="F31" s="40"/>
       <c r="G31" s="33"/>
       <c r="H31" s="24"/>
       <c r="AMJ31" s="24"/>
@@ -1382,7 +1361,7 @@
       <c r="A32" s="29" t="n">
         <v>2</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="38" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="30"/>
@@ -1395,11 +1374,11 @@
       <c r="A33" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="38" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="30"/>
-      <c r="F33" s="42"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="33"/>
       <c r="H33" s="24"/>
       <c r="AMJ33" s="24"/>
@@ -1412,7 +1391,7 @@
         <v>53</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="33"/>
@@ -1423,7 +1402,7 @@
       <c r="A35" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="30"/>
@@ -1440,9 +1419,8 @@
         <v>55</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="44"/>
+        <v>45</v>
+      </c>
       <c r="G36" s="33"/>
       <c r="H36" s="24"/>
       <c r="AMJ36" s="24"/>
@@ -1451,11 +1429,11 @@
       <c r="A37" s="29" t="n">
         <v>7</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="38" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="30"/>
-      <c r="F37" s="42"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="33"/>
       <c r="H37" s="24"/>
       <c r="AMJ37" s="24"/>
@@ -1464,7 +1442,7 @@
       <c r="A38" s="29" t="n">
         <v>8</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="38" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="30"/>
@@ -1477,7 +1455,7 @@
       <c r="A39" s="29" t="n">
         <v>9</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="31" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="30"/>
@@ -1494,9 +1472,8 @@
         <v>59</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="44"/>
+        <v>46</v>
+      </c>
       <c r="G40" s="33"/>
       <c r="H40" s="24"/>
       <c r="AMJ40" s="24"/>
@@ -1505,11 +1482,10 @@
       <c r="A41" s="29" t="n">
         <v>11</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="38" t="s">
         <v>60</v>
       </c>
       <c r="C41" s="30"/>
-      <c r="F41" s="44"/>
       <c r="G41" s="33"/>
       <c r="H41" s="24"/>
       <c r="AMJ41" s="24"/>
@@ -1518,11 +1494,10 @@
       <c r="A42" s="29" t="n">
         <v>12</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="30"/>
-      <c r="F42" s="44"/>
       <c r="G42" s="33"/>
       <c r="H42" s="24"/>
       <c r="AMJ42" s="24"/>
@@ -1531,11 +1506,11 @@
       <c r="A43" s="29" t="n">
         <v>13</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="31" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="30"/>
-      <c r="F43" s="42"/>
+      <c r="F43" s="40"/>
       <c r="G43" s="33"/>
       <c r="H43" s="24"/>
       <c r="AMJ43" s="24"/>
@@ -1544,7 +1519,7 @@
       <c r="A44" s="29" t="n">
         <v>14</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="31" t="s">
         <v>63</v>
       </c>
       <c r="C44" s="30"/>
@@ -1557,7 +1532,7 @@
       <c r="A45" s="29" t="n">
         <v>15</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="31" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="30"/>
@@ -1583,7 +1558,7 @@
       <c r="A47" s="29" t="n">
         <v>17</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="38" t="s">
         <v>67</v>
       </c>
       <c r="C47" s="30"/>
@@ -1596,7 +1571,7 @@
       <c r="A48" s="29" t="n">
         <v>18</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="38" t="s">
         <v>68</v>
       </c>
       <c r="C48" s="31"/>
@@ -1612,14 +1587,11 @@
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="0"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
       <c r="F50" s="24"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="0"/>
-      <c r="C51" s="44"/>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
@@ -1628,7 +1600,6 @@
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="0"/>
-      <c r="C52" s="44"/>
       <c r="D52" s="24"/>
       <c r="E52" s="24"/>
       <c r="F52" s="24"/>
@@ -1637,7 +1608,6 @@
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0"/>
-      <c r="C53" s="44"/>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
@@ -1646,7 +1616,6 @@
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="0"/>
-      <c r="C54" s="44"/>
       <c r="D54" s="24"/>
       <c r="E54" s="24"/>
       <c r="F54" s="24"/>
@@ -1655,7 +1624,6 @@
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
       <c r="B55" s="0"/>
-      <c r="C55" s="44"/>
       <c r="D55" s="24"/>
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
@@ -1664,7 +1632,6 @@
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0"/>
       <c r="B56" s="0"/>
-      <c r="C56" s="44"/>
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
       <c r="AMJ56" s="24"/>
@@ -1672,7 +1639,6 @@
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
       <c r="B57" s="0"/>
-      <c r="C57" s="44"/>
       <c r="D57" s="24"/>
       <c r="E57" s="24"/>
       <c r="AMJ57" s="24"/>
@@ -1680,7 +1646,6 @@
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0"/>
       <c r="B58" s="0"/>
-      <c r="C58" s="44"/>
       <c r="D58" s="24"/>
       <c r="E58" s="24"/>
       <c r="AMJ58" s="24"/>
@@ -1688,37 +1653,31 @@
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
       <c r="B59" s="0"/>
-      <c r="C59" s="44"/>
       <c r="AMJ59" s="24"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="0"/>
-      <c r="C60" s="44"/>
       <c r="AMJ60" s="24"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
       <c r="B61" s="0"/>
-      <c r="C61" s="44"/>
       <c r="AMJ61" s="24"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
       <c r="B62" s="0"/>
-      <c r="C62" s="44"/>
       <c r="AMJ62" s="24"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="0"/>
-      <c r="C63" s="44"/>
       <c r="AMJ63" s="24"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0"/>
       <c r="B64" s="0"/>
-      <c r="C64" s="44"/>
       <c r="AMJ64" s="24"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>